<commit_message>
added : tag doc
</commit_message>
<xml_diff>
--- a/public/data/db_source/tag.xlsx
+++ b/public/data/db_source/tag.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E241FA8C-36A0-0C4A-AAB8-A60F09911BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B14F382-0232-9941-910B-A3FA9A5A4618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="127">
   <si>
     <t>id</t>
   </si>
@@ -473,6 +473,15 @@
   </si>
   <si>
     <t>Images aériennes</t>
+  </si>
+  <si>
+    <t>doc_ids</t>
+  </si>
+  <si>
+    <t>pdf_online</t>
+  </si>
+  <si>
+    <t>pdf_online, bevnat_info</t>
   </si>
 </sst>
 </file>
@@ -523,7 +532,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -556,13 +568,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C32CA667-C9A5-3946-BF15-6447F33C3523}" name="Tableau1" displayName="Tableau1" ref="A1:D42" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D42" xr:uid="{C32CA667-C9A5-3946-BF15-6447F33C3523}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F6FEC23F-8D10-4D47-AAA0-00D8F20EF27F}" name="id" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{D3276B84-4B67-5647-915F-15C6658C630C}" name="parent_id" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{024BB92A-5ABB-084F-BE61-A61103EB3253}" name="name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{03C0557E-C044-D74A-80B6-7703E63ADC59}" name="description" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C32CA667-C9A5-3946-BF15-6447F33C3523}" name="Tableau1" displayName="Tableau1" ref="A1:E42" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E42" xr:uid="{C32CA667-C9A5-3946-BF15-6447F33C3523}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F6FEC23F-8D10-4D47-AAA0-00D8F20EF27F}" name="id" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{D3276B84-4B67-5647-915F-15C6658C630C}" name="parent_id" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{024BB92A-5ABB-084F-BE61-A61103EB3253}" name="name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{03C0557E-C044-D74A-80B6-7703E63ADC59}" name="description" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00E2B9A6-C612-9C45-A9A7-D399C9AF52FD}" name="doc_ids" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -855,11 +868,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -868,9 +881,10 @@
     <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,8 +897,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -894,8 +911,9 @@
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -905,8 +923,9 @@
       <c r="D3" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -919,8 +938,9 @@
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -933,8 +953,11 @@
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -947,8 +970,9 @@
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -961,8 +985,9 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -975,8 +1000,11 @@
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="E8" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -989,8 +1017,9 @@
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="175" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="175" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1003,8 +1032,9 @@
       <c r="D10" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1017,8 +1047,9 @@
       <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="199" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="199" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1031,8 +1062,9 @@
       <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="200" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1045,8 +1077,9 @@
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="156" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1059,8 +1092,9 @@
       <c r="D14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="185" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="185" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1073,8 +1107,9 @@
       <c r="D15" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1087,8 +1122,9 @@
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -1101,8 +1137,9 @@
       <c r="D17" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1115,8 +1152,9 @@
       <c r="D18" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -1129,8 +1167,9 @@
       <c r="D19" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -1143,8 +1182,9 @@
       <c r="D20" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
@@ -1157,8 +1197,9 @@
       <c r="D21" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="225" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
@@ -1171,8 +1212,9 @@
       <c r="D22" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="249" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="249" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
@@ -1185,8 +1227,9 @@
       <c r="D23" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1199,8 +1242,9 @@
       <c r="D24" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="228" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="228" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
@@ -1213,8 +1257,9 @@
       <c r="D25" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
@@ -1227,8 +1272,9 @@
       <c r="D26" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>67</v>
       </c>
@@ -1241,8 +1287,9 @@
       <c r="D27" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
@@ -1255,8 +1302,9 @@
       <c r="D28" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>73</v>
       </c>
@@ -1269,8 +1317,9 @@
       <c r="D29" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>75</v>
       </c>
@@ -1283,8 +1332,9 @@
       <c r="D30" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="188" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="188" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>77</v>
       </c>
@@ -1297,8 +1347,9 @@
       <c r="D31" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
@@ -1311,8 +1362,9 @@
       <c r="D32" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -1325,8 +1377,9 @@
       <c r="D33" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>84</v>
       </c>
@@ -1339,8 +1392,9 @@
       <c r="D34" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>87</v>
       </c>
@@ -1353,8 +1407,9 @@
       <c r="D35" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="228" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="228" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>89</v>
       </c>
@@ -1367,8 +1422,9 @@
       <c r="D36" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>92</v>
       </c>
@@ -1381,8 +1437,9 @@
       <c r="D37" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>95</v>
       </c>
@@ -1395,8 +1452,9 @@
       <c r="D38" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>97</v>
       </c>
@@ -1409,8 +1467,9 @@
       <c r="D39" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>100</v>
       </c>
@@ -1423,8 +1482,9 @@
       <c r="D40" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>102</v>
       </c>
@@ -1437,6 +1497,10 @@
       <c r="D41" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>